<commit_message>
Changed start up message, start up workflow in progress
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dswindle\OneDrive - Capgemini\Documents\DEFRA\UiPath-Templates\Attended Process Template\Documents\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD9F8128-AD06-4CC0-AE67-130C5FE388F8}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4BF8A0-CBBF-436C-A6FA-4B0CDBE7B9B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
   <si>
     <t>Name</t>
   </si>
@@ -40,6 +40,168 @@
   </si>
   <si>
     <t>Regex</t>
+  </si>
+  <si>
+    <t>LogFilePath</t>
+  </si>
+  <si>
+    <t>File Path for log file</t>
+  </si>
+  <si>
+    <t>C:\Users\{0}\Desktop\FFCP Logs_{1}.xlsx</t>
+  </si>
+  <si>
+    <t>Path for Robot Processing Folder</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9)Processing Folders\Robot</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\CII Receipting</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\Master Copies</t>
+  </si>
+  <si>
+    <t>RobotProcessingFolder</t>
+  </si>
+  <si>
+    <t>CIIReceiptingFolder</t>
+  </si>
+  <si>
+    <t>AwaitingARFFolder</t>
+  </si>
+  <si>
+    <t>MasterCopiesFolder</t>
+  </si>
+  <si>
+    <t>BPSCToBeAssignedFolder</t>
+  </si>
+  <si>
+    <t>BPSNCToBeAssignedFolder</t>
+  </si>
+  <si>
+    <t>NonBPSCToBeAssignedFolder</t>
+  </si>
+  <si>
+    <t>NonBPSNCToBeAssignedFolder</t>
+  </si>
+  <si>
+    <t>ARFFolder</t>
+  </si>
+  <si>
+    <t>ARFMatchedFolder</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\Master Copies\CII\CRF's &amp; ARF's matched</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\Master Copies\CII\Awaiting ARF</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\Master Copies\CII\ARF's</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\3) Non BPS NC to be assigned</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\4) Non BPS C to be assigned</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\1) BPS NC to be assigned</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\2) BPS C to be assigned</t>
+  </si>
+  <si>
+    <t>FilePaths</t>
+  </si>
+  <si>
+    <t>URLs</t>
+  </si>
+  <si>
+    <t>CRMUrl</t>
+  </si>
+  <si>
+    <t>Url for CRM</t>
+  </si>
+  <si>
+    <t>Path for CII Receipting Folder</t>
+  </si>
+  <si>
+    <t>Path for Master Copies Folder</t>
+  </si>
+  <si>
+    <t>Path for BPS Compliant To Be Assigned Folder</t>
+  </si>
+  <si>
+    <t>Path for BPS Non-Compliant To Be Assigned Folder</t>
+  </si>
+  <si>
+    <t>Path for Non BPS Compliant To Be Assigned Folder</t>
+  </si>
+  <si>
+    <t>Path for Non BPS Non-Compliant To Be Assigned Folder</t>
+  </si>
+  <si>
+    <t>Path for ARF Folder where new ARFs are saved.</t>
+  </si>
+  <si>
+    <t>Path for Awaiting ARF Folder where CRFs without matching ARFs are saved</t>
+  </si>
+  <si>
+    <t>Path for ARF Matched Folder where SBI folders containing a matching ARF and CRF are placed for Master Copy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://rpa-csc-uat.crm4.dynamics.com/main.aspx                                                        </t>
+  </si>
+  <si>
+    <t>Timeouts</t>
+  </si>
+  <si>
+    <t>timeoutM</t>
+  </si>
+  <si>
+    <t>timeoutS</t>
+  </si>
+  <si>
+    <t>timeoutXS</t>
+  </si>
+  <si>
+    <t>timeoutL</t>
+  </si>
+  <si>
+    <t>timeoutXL</t>
+  </si>
+  <si>
+    <t>timeoutMS</t>
+  </si>
+  <si>
+    <t>2 minutes</t>
+  </si>
+  <si>
+    <t>1 minute</t>
+  </si>
+  <si>
+    <t>30 seconds</t>
+  </si>
+  <si>
+    <t>5 seconds</t>
+  </si>
+  <si>
+    <t>3 seconds</t>
+  </si>
+  <si>
+    <t>1 second</t>
+  </si>
+  <si>
+    <t>RPHomeUrl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ruralpayments.service.gov.uk/login </t>
+  </si>
+  <si>
+    <t>Url for Rural Payments homepage</t>
   </si>
 </sst>
 </file>
@@ -93,7 +255,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -116,6 +278,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -165,8 +331,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C5" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C5" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C29" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
@@ -473,15 +639,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C29"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+      <selection activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.7109375" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.7109375" style="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="69" style="4" customWidth="1"/>
     <col min="3" max="3" width="38" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="16384" width="9.140625" style="3"/>
@@ -505,14 +671,244 @@
       <c r="B2" s="2"/>
       <c r="C2" s="2"/>
     </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="5" t="s">
+        <v>43</v>
+      </c>
+      <c r="B3" s="2"/>
+      <c r="C3" s="2"/>
+    </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="5" t="s">
+      <c r="A4" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B4" s="4">
+        <v>1000</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B5" s="4">
+        <v>3000</v>
+      </c>
+      <c r="C5" s="8" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B6" s="4">
+        <v>5000</v>
+      </c>
+      <c r="C6" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B7" s="4">
+        <v>30000</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B8" s="4">
+        <v>60000</v>
+      </c>
+      <c r="C8" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B9" s="4">
+        <v>120000</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B10" s="2"/>
+      <c r="C10" s="2"/>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B11" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="2"/>
+      <c r="C13" s="2"/>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A14" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B14" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="C14" s="4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B15" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C15" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B17" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C17" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B18" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C18" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A19" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B22" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="6"/>
-      <c r="B5" s="7"/>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="6"/>
+      <c r="B29" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Created Siti library, finished Open RP
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D4BF8A0-CBBF-436C-A6FA-4B0CDBE7B9B2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85493D2C-241A-4332-AD66-21999D35647F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="15" yWindow="1485" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
   <si>
     <t>Name</t>
   </si>
@@ -202,6 +202,27 @@
   </si>
   <si>
     <t>Url for Rural Payments homepage</t>
+  </si>
+  <si>
+    <t>maxRetries</t>
+  </si>
+  <si>
+    <t>RPLogInUrl</t>
+  </si>
+  <si>
+    <t>https://www.ruralpayments.service.gov.uk/#/internal_user/main</t>
+  </si>
+  <si>
+    <t>SitiAgriUrl</t>
+  </si>
+  <si>
+    <t>https://www.ruralpayments.service.gov.uk/sitiAgriMenu/</t>
+  </si>
+  <si>
+    <t>Url for Rural Payments Log in Page</t>
+  </si>
+  <si>
+    <t>Url for SitiAgri</t>
   </si>
 </sst>
 </file>
@@ -331,8 +352,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C29" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C29" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C32" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
@@ -639,10 +660,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C29"/>
+  <dimension ref="A1:C32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -680,235 +701,266 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
-        <v>46</v>
+        <v>59</v>
       </c>
       <c r="B4" s="4">
-        <v>1000</v>
-      </c>
-      <c r="C4" s="8" t="s">
-        <v>55</v>
-      </c>
+        <v>3</v>
+      </c>
+      <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
       <c r="B5" s="4">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>54</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="3" t="s">
-        <v>45</v>
+        <v>49</v>
       </c>
       <c r="B6" s="4">
-        <v>5000</v>
+        <v>3000</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="B7" s="4">
-        <v>30000</v>
+        <v>5000</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
       <c r="B8" s="4">
-        <v>60000</v>
+        <v>30000</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>51</v>
+        <v>52</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B9" s="4">
+        <v>60000</v>
+      </c>
+      <c r="C9" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B9" s="4">
+      <c r="B10" s="4">
         <v>120000</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C10" s="8" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="5" t="s">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A11" s="5" t="s">
         <v>30</v>
       </c>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B11" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C11" s="8" t="s">
-        <v>32</v>
-      </c>
+      <c r="B11" s="2"/>
+      <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>56</v>
+        <v>31</v>
       </c>
       <c r="B12" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C12" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A13" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B13" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="C12" s="8" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A13" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
+      <c r="C13" s="8" t="s">
+        <v>64</v>
+      </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C14" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A15" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B15" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C15" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A16" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="2"/>
+      <c r="C16" s="2"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A17" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="4" t="s">
+      <c r="B17" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C14" s="4" t="s">
+      <c r="C17" s="4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B15" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C15" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B16" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="17" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A17" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B17" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C17" s="4" t="s">
-        <v>34</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>28</v>
+        <v>9</v>
       </c>
       <c r="C18" s="4" t="s">
-        <v>35</v>
+        <v>8</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C19" s="4" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>26</v>
+        <v>11</v>
       </c>
       <c r="C20" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
     </row>
     <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="C22" s="4" t="s">
-        <v>39</v>
+        <v>36</v>
       </c>
     </row>
     <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A24" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B25" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B23" s="4" t="s">
+      <c r="B26" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C23" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
+    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B24" s="4" t="s">
+      <c r="B27" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C27" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="5" t="s">
+    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A31" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" s="6"/>
-      <c r="B29" s="7"/>
+    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A32" s="6"/>
+      <c r="B32" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added logic for opening Siti Agri, published Siti Library, Started validation
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85493D2C-241A-4332-AD66-21999D35647F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E05750-60AA-4937-A13D-E5E5097B2BF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="1485" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -663,7 +663,7 @@
   <dimension ref="A1:C32"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
added changes to populate queue with breakpoint logix
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x952359$\Development\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E05750-60AA-4937-A13D-E5E5097B2BF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
   <si>
     <t>Name</t>
   </si>
@@ -223,12 +222,90 @@
   </si>
   <si>
     <t>Url for SitiAgri</t>
+  </si>
+  <si>
+    <t>MailBoxes</t>
+  </si>
+  <si>
+    <t>SAGMailbox</t>
+  </si>
+  <si>
+    <t>RPAMailbox</t>
+  </si>
+  <si>
+    <t>AHMailbox</t>
+  </si>
+  <si>
+    <t>CiiMailbox</t>
+  </si>
+  <si>
+    <t>SAGReports.XC@rpa.gov.uk</t>
+  </si>
+  <si>
+    <t>XCAnimalHealthStandaloneandselected@rpa.gov.uk</t>
+  </si>
+  <si>
+    <t>XCRPAreports@rpa.gov.uk</t>
+  </si>
+  <si>
+    <t>CrossCompliance.DiscrepancyReports@rpa.gov.uk</t>
+  </si>
+  <si>
+    <t>inProgressFolder</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Supervision Mode</t>
+  </si>
+  <si>
+    <t>boolSupervision</t>
+  </si>
+  <si>
+    <t>boolControlPoint1</t>
+  </si>
+  <si>
+    <t>boolControlPoint2</t>
+  </si>
+  <si>
+    <t>boolControlPoint3</t>
+  </si>
+  <si>
+    <t>boolControlPoint4</t>
+  </si>
+  <si>
+    <t>boolControlPoint5</t>
+  </si>
+  <si>
+    <t>boolControlPoint6</t>
+  </si>
+  <si>
+    <t>master switch for high low supervision</t>
+  </si>
+  <si>
+    <t>switch for breakpoint 1</t>
+  </si>
+  <si>
+    <t>switch for breakpoint 2</t>
+  </si>
+  <si>
+    <t>switch for breakpoint 3</t>
+  </si>
+  <si>
+    <t>switch for breakpoint 4</t>
+  </si>
+  <si>
+    <t>switch for breakpoint 5</t>
+  </si>
+  <si>
+    <t>switch for breakpoint 6</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -352,12 +429,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C32" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C32" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C43" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C43"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="2"/>
+    <tableColumn id="2" name="Value" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -659,11 +736,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C32"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="A26" sqref="A26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -694,273 +771,402 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>43</v>
+        <v>77</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>59</v>
-      </c>
-      <c r="B4" s="4">
-        <v>3</v>
-      </c>
-      <c r="C4" s="2"/>
+      <c r="A4" s="6" t="s">
+        <v>78</v>
+      </c>
+      <c r="B4" s="8" t="b">
+        <v>1</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B5" s="4">
-        <v>1000</v>
+      <c r="A5" s="6" t="s">
+        <v>79</v>
+      </c>
+      <c r="B5" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>55</v>
+        <v>86</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B6" s="4">
-        <v>3000</v>
+      <c r="A6" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B6" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>54</v>
+        <v>87</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B7" s="4">
-        <v>5000</v>
+      <c r="A7" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="B7" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>53</v>
+        <v>88</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B8" s="4">
-        <v>30000</v>
+      <c r="A8" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="B8" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>52</v>
+        <v>89</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B9" s="4">
-        <v>60000</v>
+      <c r="A9" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="B9" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>51</v>
+        <v>90</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B10" s="4">
-        <v>120000</v>
+      <c r="A10" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B10" s="8" t="b">
+        <v>1</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>30</v>
+        <v>43</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B12" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C12" s="8" t="s">
-        <v>32</v>
-      </c>
+        <v>59</v>
+      </c>
+      <c r="B12" s="4">
+        <v>3</v>
+      </c>
+      <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>60</v>
-      </c>
-      <c r="B13" s="9" t="s">
-        <v>57</v>
+        <v>46</v>
+      </c>
+      <c r="B13" s="4">
+        <v>1000</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="B14" s="9" t="s">
-        <v>61</v>
+        <v>49</v>
+      </c>
+      <c r="B14" s="4">
+        <v>3000</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>58</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>62</v>
-      </c>
-      <c r="B15" s="9" t="s">
-        <v>63</v>
+        <v>45</v>
+      </c>
+      <c r="B15" s="4">
+        <v>5000</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>65</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A16" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
+      <c r="A16" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="4">
+        <v>30000</v>
+      </c>
+      <c r="C16" s="8" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="4">
+        <v>60000</v>
+      </c>
+      <c r="C17" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A18" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="4">
+        <v>120000</v>
+      </c>
+      <c r="C18" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A19" s="5" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="2"/>
+      <c r="C19" s="2"/>
+    </row>
+    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A20" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>42</v>
+      </c>
+      <c r="C20" s="8" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A21" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="B21" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" s="8" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A22" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="B22" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="B23" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="C23" s="8" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A24" s="5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B24" s="2"/>
+      <c r="C24" s="2"/>
+    </row>
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A25" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B17" s="4" t="s">
+      <c r="B25" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C17" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="18" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A18" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B18" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C18" s="4" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="19" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A19" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C19" s="4" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="20" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A20" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" s="4" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="21" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C21" s="4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A22" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="23" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="24" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="C24" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A25" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C25" s="4" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B26" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C26" s="4" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B28" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C28" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B29" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="C29" s="4" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A30" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B30" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="C30" s="4" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B31" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C31" s="4" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A32" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B32" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="C32" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A33" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B33" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C33" s="4" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A34" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B26" s="4" t="s">
+      <c r="B34" s="4" t="s">
         <v>23</v>
       </c>
-      <c r="C26" s="4" t="s">
+      <c r="C34" s="4" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="27" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+    <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A35" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B35" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C35" s="4" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A36" s="5" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A37" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="B38" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" s="6"/>
-      <c r="B32" s="7"/>
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A43" s="6"/>
+      <c r="B43" s="7"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
adding new crf location file
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -53,253 +53,253 @@
     <t>Path for Robot Processing Folder</t>
   </si>
   <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\CII Receipting</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\Master Copies</t>
+  </si>
+  <si>
+    <t>RobotProcessingFolder</t>
+  </si>
+  <si>
+    <t>CIIReceiptingFolder</t>
+  </si>
+  <si>
+    <t>AwaitingARFFolder</t>
+  </si>
+  <si>
+    <t>MasterCopiesFolder</t>
+  </si>
+  <si>
+    <t>BPSCToBeAssignedFolder</t>
+  </si>
+  <si>
+    <t>BPSNCToBeAssignedFolder</t>
+  </si>
+  <si>
+    <t>NonBPSCToBeAssignedFolder</t>
+  </si>
+  <si>
+    <t>NonBPSNCToBeAssignedFolder</t>
+  </si>
+  <si>
+    <t>ARFFolder</t>
+  </si>
+  <si>
+    <t>ARFMatchedFolder</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\Master Copies\CII\CRF's &amp; ARF's matched</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\Master Copies\CII\Awaiting ARF</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\Master Copies\CII\ARF's</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\3) Non BPS NC to be assigned</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\4) Non BPS C to be assigned</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\1) BPS NC to be assigned</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\2) BPS C to be assigned</t>
+  </si>
+  <si>
+    <t>FilePaths</t>
+  </si>
+  <si>
+    <t>URLs</t>
+  </si>
+  <si>
+    <t>CRMUrl</t>
+  </si>
+  <si>
+    <t>Url for CRM</t>
+  </si>
+  <si>
+    <t>Path for CII Receipting Folder</t>
+  </si>
+  <si>
+    <t>Path for Master Copies Folder</t>
+  </si>
+  <si>
+    <t>Path for BPS Compliant To Be Assigned Folder</t>
+  </si>
+  <si>
+    <t>Path for BPS Non-Compliant To Be Assigned Folder</t>
+  </si>
+  <si>
+    <t>Path for Non BPS Compliant To Be Assigned Folder</t>
+  </si>
+  <si>
+    <t>Path for Non BPS Non-Compliant To Be Assigned Folder</t>
+  </si>
+  <si>
+    <t>Path for ARF Folder where new ARFs are saved.</t>
+  </si>
+  <si>
+    <t>Path for Awaiting ARF Folder where CRFs without matching ARFs are saved</t>
+  </si>
+  <si>
+    <t>Path for ARF Matched Folder where SBI folders containing a matching ARF and CRF are placed for Master Copy.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://rpa-csc-uat.crm4.dynamics.com/main.aspx                                                        </t>
+  </si>
+  <si>
+    <t>Timeouts</t>
+  </si>
+  <si>
+    <t>timeoutM</t>
+  </si>
+  <si>
+    <t>timeoutS</t>
+  </si>
+  <si>
+    <t>timeoutXS</t>
+  </si>
+  <si>
+    <t>timeoutL</t>
+  </si>
+  <si>
+    <t>timeoutXL</t>
+  </si>
+  <si>
+    <t>timeoutMS</t>
+  </si>
+  <si>
+    <t>2 minutes</t>
+  </si>
+  <si>
+    <t>1 minute</t>
+  </si>
+  <si>
+    <t>30 seconds</t>
+  </si>
+  <si>
+    <t>5 seconds</t>
+  </si>
+  <si>
+    <t>3 seconds</t>
+  </si>
+  <si>
+    <t>1 second</t>
+  </si>
+  <si>
+    <t>RPHomeUrl</t>
+  </si>
+  <si>
+    <t xml:space="preserve">https://www.ruralpayments.service.gov.uk/login </t>
+  </si>
+  <si>
+    <t>Url for Rural Payments homepage</t>
+  </si>
+  <si>
+    <t>maxRetries</t>
+  </si>
+  <si>
+    <t>RPLogInUrl</t>
+  </si>
+  <si>
+    <t>https://www.ruralpayments.service.gov.uk/#/internal_user/main</t>
+  </si>
+  <si>
+    <t>SitiAgriUrl</t>
+  </si>
+  <si>
+    <t>https://www.ruralpayments.service.gov.uk/sitiAgriMenu/</t>
+  </si>
+  <si>
+    <t>Url for Rural Payments Log in Page</t>
+  </si>
+  <si>
+    <t>Url for SitiAgri</t>
+  </si>
+  <si>
+    <t>MailBoxes</t>
+  </si>
+  <si>
+    <t>SAGMailbox</t>
+  </si>
+  <si>
+    <t>RPAMailbox</t>
+  </si>
+  <si>
+    <t>AHMailbox</t>
+  </si>
+  <si>
+    <t>CiiMailbox</t>
+  </si>
+  <si>
+    <t>SAGReports.XC@rpa.gov.uk</t>
+  </si>
+  <si>
+    <t>XCAnimalHealthStandaloneandselected@rpa.gov.uk</t>
+  </si>
+  <si>
+    <t>XCRPAreports@rpa.gov.uk</t>
+  </si>
+  <si>
+    <t>CrossCompliance.DiscrepancyReports@rpa.gov.uk</t>
+  </si>
+  <si>
+    <t>inProgressFolder</t>
+  </si>
+  <si>
+    <t>In Progress</t>
+  </si>
+  <si>
+    <t>Supervision Mode</t>
+  </si>
+  <si>
+    <t>boolSupervision</t>
+  </si>
+  <si>
+    <t>boolControlPoint1</t>
+  </si>
+  <si>
+    <t>boolControlPoint2</t>
+  </si>
+  <si>
+    <t>boolControlPoint3</t>
+  </si>
+  <si>
+    <t>boolControlPoint4</t>
+  </si>
+  <si>
+    <t>boolControlPoint5</t>
+  </si>
+  <si>
+    <t>boolControlPoint6</t>
+  </si>
+  <si>
+    <t>master switch for high low supervision</t>
+  </si>
+  <si>
+    <t>switch for breakpoint 1</t>
+  </si>
+  <si>
+    <t>switch for breakpoint 2</t>
+  </si>
+  <si>
+    <t>switch for breakpoint 3</t>
+  </si>
+  <si>
+    <t>switch for breakpoint 4</t>
+  </si>
+  <si>
+    <t>switch for breakpoint 5</t>
+  </si>
+  <si>
+    <t>switch for breakpoint 6</t>
+  </si>
+  <si>
     <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9)Processing Folders\Robot</t>
-  </si>
-  <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\CII Receipting</t>
-  </si>
-  <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\Master Copies</t>
-  </si>
-  <si>
-    <t>RobotProcessingFolder</t>
-  </si>
-  <si>
-    <t>CIIReceiptingFolder</t>
-  </si>
-  <si>
-    <t>AwaitingARFFolder</t>
-  </si>
-  <si>
-    <t>MasterCopiesFolder</t>
-  </si>
-  <si>
-    <t>BPSCToBeAssignedFolder</t>
-  </si>
-  <si>
-    <t>BPSNCToBeAssignedFolder</t>
-  </si>
-  <si>
-    <t>NonBPSCToBeAssignedFolder</t>
-  </si>
-  <si>
-    <t>NonBPSNCToBeAssignedFolder</t>
-  </si>
-  <si>
-    <t>ARFFolder</t>
-  </si>
-  <si>
-    <t>ARFMatchedFolder</t>
-  </si>
-  <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\Master Copies\CII\CRF's &amp; ARF's matched</t>
-  </si>
-  <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\Master Copies\CII\Awaiting ARF</t>
-  </si>
-  <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\Master Copies\CII\ARF's</t>
-  </si>
-  <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\3) Non BPS NC to be assigned</t>
-  </si>
-  <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\4) Non BPS C to be assigned</t>
-  </si>
-  <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\1) BPS NC to be assigned</t>
-  </si>
-  <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\2) BPS C to be assigned</t>
-  </si>
-  <si>
-    <t>FilePaths</t>
-  </si>
-  <si>
-    <t>URLs</t>
-  </si>
-  <si>
-    <t>CRMUrl</t>
-  </si>
-  <si>
-    <t>Url for CRM</t>
-  </si>
-  <si>
-    <t>Path for CII Receipting Folder</t>
-  </si>
-  <si>
-    <t>Path for Master Copies Folder</t>
-  </si>
-  <si>
-    <t>Path for BPS Compliant To Be Assigned Folder</t>
-  </si>
-  <si>
-    <t>Path for BPS Non-Compliant To Be Assigned Folder</t>
-  </si>
-  <si>
-    <t>Path for Non BPS Compliant To Be Assigned Folder</t>
-  </si>
-  <si>
-    <t>Path for Non BPS Non-Compliant To Be Assigned Folder</t>
-  </si>
-  <si>
-    <t>Path for ARF Folder where new ARFs are saved.</t>
-  </si>
-  <si>
-    <t>Path for Awaiting ARF Folder where CRFs without matching ARFs are saved</t>
-  </si>
-  <si>
-    <t>Path for ARF Matched Folder where SBI folders containing a matching ARF and CRF are placed for Master Copy.</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://rpa-csc-uat.crm4.dynamics.com/main.aspx                                                        </t>
-  </si>
-  <si>
-    <t>Timeouts</t>
-  </si>
-  <si>
-    <t>timeoutM</t>
-  </si>
-  <si>
-    <t>timeoutS</t>
-  </si>
-  <si>
-    <t>timeoutXS</t>
-  </si>
-  <si>
-    <t>timeoutL</t>
-  </si>
-  <si>
-    <t>timeoutXL</t>
-  </si>
-  <si>
-    <t>timeoutMS</t>
-  </si>
-  <si>
-    <t>2 minutes</t>
-  </si>
-  <si>
-    <t>1 minute</t>
-  </si>
-  <si>
-    <t>30 seconds</t>
-  </si>
-  <si>
-    <t>5 seconds</t>
-  </si>
-  <si>
-    <t>3 seconds</t>
-  </si>
-  <si>
-    <t>1 second</t>
-  </si>
-  <si>
-    <t>RPHomeUrl</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://www.ruralpayments.service.gov.uk/login </t>
-  </si>
-  <si>
-    <t>Url for Rural Payments homepage</t>
-  </si>
-  <si>
-    <t>maxRetries</t>
-  </si>
-  <si>
-    <t>RPLogInUrl</t>
-  </si>
-  <si>
-    <t>https://www.ruralpayments.service.gov.uk/#/internal_user/main</t>
-  </si>
-  <si>
-    <t>SitiAgriUrl</t>
-  </si>
-  <si>
-    <t>https://www.ruralpayments.service.gov.uk/sitiAgriMenu/</t>
-  </si>
-  <si>
-    <t>Url for Rural Payments Log in Page</t>
-  </si>
-  <si>
-    <t>Url for SitiAgri</t>
-  </si>
-  <si>
-    <t>MailBoxes</t>
-  </si>
-  <si>
-    <t>SAGMailbox</t>
-  </si>
-  <si>
-    <t>RPAMailbox</t>
-  </si>
-  <si>
-    <t>AHMailbox</t>
-  </si>
-  <si>
-    <t>CiiMailbox</t>
-  </si>
-  <si>
-    <t>SAGReports.XC@rpa.gov.uk</t>
-  </si>
-  <si>
-    <t>XCAnimalHealthStandaloneandselected@rpa.gov.uk</t>
-  </si>
-  <si>
-    <t>XCRPAreports@rpa.gov.uk</t>
-  </si>
-  <si>
-    <t>CrossCompliance.DiscrepancyReports@rpa.gov.uk</t>
-  </si>
-  <si>
-    <t>inProgressFolder</t>
-  </si>
-  <si>
-    <t>In Progress</t>
-  </si>
-  <si>
-    <t>Supervision Mode</t>
-  </si>
-  <si>
-    <t>boolSupervision</t>
-  </si>
-  <si>
-    <t>boolControlPoint1</t>
-  </si>
-  <si>
-    <t>boolControlPoint2</t>
-  </si>
-  <si>
-    <t>boolControlPoint3</t>
-  </si>
-  <si>
-    <t>boolControlPoint4</t>
-  </si>
-  <si>
-    <t>boolControlPoint5</t>
-  </si>
-  <si>
-    <t>boolControlPoint6</t>
-  </si>
-  <si>
-    <t>master switch for high low supervision</t>
-  </si>
-  <si>
-    <t>switch for breakpoint 1</t>
-  </si>
-  <si>
-    <t>switch for breakpoint 2</t>
-  </si>
-  <si>
-    <t>switch for breakpoint 3</t>
-  </si>
-  <si>
-    <t>switch for breakpoint 4</t>
-  </si>
-  <si>
-    <t>switch for breakpoint 5</t>
-  </si>
-  <si>
-    <t>switch for breakpoint 6</t>
   </si>
 </sst>
 </file>
@@ -739,8 +739,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C43"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -771,98 +771,98 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B3" s="2"/>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B4" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C4" s="8" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B5" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C5" s="8" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B6" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C6" s="8" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B7" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C7" s="8" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B8" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B9" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B10" s="8" t="b">
         <v>1</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B11" s="2"/>
       <c r="C11" s="2"/>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B12" s="4">
         <v>3</v>
@@ -871,124 +871,124 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B13" s="4">
         <v>1000</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B14" s="4">
         <v>3000</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B15" s="4">
         <v>5000</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B16" s="4">
         <v>30000</v>
       </c>
       <c r="C16" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B17" s="4">
         <v>60000</v>
       </c>
       <c r="C17" s="8" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B18" s="4">
         <v>120000</v>
       </c>
       <c r="C18" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="C20" s="8" t="s">
         <v>31</v>
-      </c>
-      <c r="B20" s="9" t="s">
-        <v>42</v>
-      </c>
-      <c r="C20" s="8" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B21" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C21" s="8" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B22" s="9" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C22" s="8" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="9" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="9" t="s">
-        <v>63</v>
-      </c>
       <c r="C23" s="8" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B24" s="2"/>
       <c r="C24" s="2"/>
@@ -1006,10 +1006,10 @@
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>9</v>
+        <v>91</v>
       </c>
       <c r="C26" s="4" t="s">
         <v>8</v>
@@ -1017,146 +1017,146 @@
     </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C27" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A28" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C28" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B35" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B35" s="4" t="s">
-        <v>22</v>
-      </c>
       <c r="C35" s="4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="5" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B41" s="4" t="s">
         <v>75</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>76</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Created ahtb workflow, added to aw, put details in config
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x952359$\Development\rpa-future-farming-cross-compliance\Documents\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{985D29E4-2EAF-4460-98EF-CF3992E24F9E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="92">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="108">
   <si>
     <t>Name</t>
   </si>
@@ -300,12 +301,60 @@
   </si>
   <si>
     <t>switch for breakpoint 6</t>
+  </si>
+  <si>
+    <t>ahtbCPH</t>
+  </si>
+  <si>
+    <t>CPH\s*(\d{2}\/\d{3}\/\d{4})</t>
+  </si>
+  <si>
+    <t>ahtbDate</t>
+  </si>
+  <si>
+    <t>Date\s*breach\s*identified\s*((\d{2}(\/|-|.)){2}\d{4})</t>
+  </si>
+  <si>
+    <t>awSBI</t>
+  </si>
+  <si>
+    <t>awCPH</t>
+  </si>
+  <si>
+    <t>awInspectionEndDate</t>
+  </si>
+  <si>
+    <t>awNoticeGiven</t>
+  </si>
+  <si>
+    <t>awInspectorName</t>
+  </si>
+  <si>
+    <t>awSMR</t>
+  </si>
+  <si>
+    <t>(11|12|13)\s{2}\d{2}\/\d{3}\/\d{4}</t>
+  </si>
+  <si>
+    <t>Name\s{2}(\w+(\W\w+)?)</t>
+  </si>
+  <si>
+    <t>notice\sgiven\s\(hours\)\s*(\d+)</t>
+  </si>
+  <si>
+    <t>End\sdate:\s((\d{2}(\/|-|.)){2}\d{4})</t>
+  </si>
+  <si>
+    <t>\(CPH\)\snumber\s\(1\)\*\s*(\d{2}\/\d{3}\/\d{4})</t>
+  </si>
+  <si>
+    <t>\(SBI\/CRN\/BRN\)\s*(\d{9})</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -353,7 +402,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
@@ -372,9 +421,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
@@ -429,12 +475,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C43" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C43"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C50" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C50" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Name" dataDxfId="2"/>
-    <tableColumn id="2" name="Value" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -736,11 +782,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C43"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="A26" sqref="A26"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -780,10 +826,10 @@
       <c r="A4" s="6" t="s">
         <v>78</v>
       </c>
-      <c r="B4" s="8" t="b">
+      <c r="B4" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="7" t="s">
         <v>85</v>
       </c>
     </row>
@@ -791,10 +837,10 @@
       <c r="A5" s="6" t="s">
         <v>79</v>
       </c>
-      <c r="B5" s="8" t="b">
+      <c r="B5" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="7" t="s">
         <v>86</v>
       </c>
     </row>
@@ -802,10 +848,10 @@
       <c r="A6" s="6" t="s">
         <v>80</v>
       </c>
-      <c r="B6" s="8" t="b">
+      <c r="B6" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>87</v>
       </c>
     </row>
@@ -813,10 +859,10 @@
       <c r="A7" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="B7" s="8" t="b">
+      <c r="B7" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="7" t="s">
         <v>88</v>
       </c>
     </row>
@@ -824,10 +870,10 @@
       <c r="A8" s="6" t="s">
         <v>82</v>
       </c>
-      <c r="B8" s="8" t="b">
+      <c r="B8" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="7" t="s">
         <v>89</v>
       </c>
     </row>
@@ -835,10 +881,10 @@
       <c r="A9" s="6" t="s">
         <v>83</v>
       </c>
-      <c r="B9" s="8" t="b">
+      <c r="B9" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="7" t="s">
         <v>90</v>
       </c>
     </row>
@@ -846,10 +892,10 @@
       <c r="A10" s="6" t="s">
         <v>84</v>
       </c>
-      <c r="B10" s="8" t="b">
+      <c r="B10" s="7" t="b">
         <v>1</v>
       </c>
-      <c r="C10" s="8" t="s">
+      <c r="C10" s="7" t="s">
         <v>91</v>
       </c>
     </row>
@@ -876,7 +922,7 @@
       <c r="B13" s="4">
         <v>1000</v>
       </c>
-      <c r="C13" s="8" t="s">
+      <c r="C13" s="7" t="s">
         <v>55</v>
       </c>
     </row>
@@ -887,7 +933,7 @@
       <c r="B14" s="4">
         <v>3000</v>
       </c>
-      <c r="C14" s="8" t="s">
+      <c r="C14" s="7" t="s">
         <v>54</v>
       </c>
     </row>
@@ -898,7 +944,7 @@
       <c r="B15" s="4">
         <v>5000</v>
       </c>
-      <c r="C15" s="8" t="s">
+      <c r="C15" s="7" t="s">
         <v>53</v>
       </c>
     </row>
@@ -909,7 +955,7 @@
       <c r="B16" s="4">
         <v>30000</v>
       </c>
-      <c r="C16" s="8" t="s">
+      <c r="C16" s="7" t="s">
         <v>52</v>
       </c>
     </row>
@@ -920,7 +966,7 @@
       <c r="B17" s="4">
         <v>60000</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C17" s="7" t="s">
         <v>51</v>
       </c>
     </row>
@@ -931,7 +977,7 @@
       <c r="B18" s="4">
         <v>120000</v>
       </c>
-      <c r="C18" s="8" t="s">
+      <c r="C18" s="7" t="s">
         <v>50</v>
       </c>
     </row>
@@ -946,10 +992,10 @@
       <c r="A20" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B20" s="9" t="s">
+      <c r="B20" s="8" t="s">
         <v>42</v>
       </c>
-      <c r="C20" s="8" t="s">
+      <c r="C20" s="7" t="s">
         <v>32</v>
       </c>
     </row>
@@ -957,10 +1003,10 @@
       <c r="A21" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B21" s="9" t="s">
+      <c r="B21" s="8" t="s">
         <v>57</v>
       </c>
-      <c r="C21" s="8" t="s">
+      <c r="C21" s="7" t="s">
         <v>64</v>
       </c>
     </row>
@@ -968,10 +1014,10 @@
       <c r="A22" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B22" s="9" t="s">
+      <c r="B22" s="8" t="s">
         <v>61</v>
       </c>
-      <c r="C22" s="8" t="s">
+      <c r="C22" s="7" t="s">
         <v>58</v>
       </c>
     </row>
@@ -979,10 +1025,10 @@
       <c r="A23" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B23" s="9" t="s">
+      <c r="B23" s="8" t="s">
         <v>63</v>
       </c>
-      <c r="C23" s="8" t="s">
+      <c r="C23" s="7" t="s">
         <v>65</v>
       </c>
     </row>
@@ -1165,8 +1211,68 @@
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="6"/>
-      <c r="B43" s="7"/>
+      <c r="A43" s="6" t="s">
+        <v>92</v>
+      </c>
+      <c r="B43" s="4" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A44" s="3" t="s">
+        <v>94</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B48" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>102</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
journey testing. Changed logic to include in progress + to be rreceipted folders
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C8CAC41F-B3AC-4AA2-9705-BFA23BDD2720}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EF0DECC-5827-4095-B7F7-F6FDD6D55335}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="122">
   <si>
     <t>Name</t>
   </si>
@@ -373,6 +373,24 @@
   </si>
   <si>
     <t>Future-Farming-Cross-Compliance</t>
+  </si>
+  <si>
+    <t>ReadyToBeReceiptedFolder</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9)Processing Folders\Robot\{1}\In Progress\</t>
+  </si>
+  <si>
+    <t>InProgressWindowFolder</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9)Processing Folders\Robot\{1}\Ready To Be Receipted\</t>
+  </si>
+  <si>
+    <t>in progress path for all crf types</t>
+  </si>
+  <si>
+    <t>ready to be receipted for all crf types - use for deployment 1 only</t>
   </si>
 </sst>
 </file>
@@ -502,8 +520,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C53" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C53" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C55" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C55" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
@@ -810,10 +828,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C53"/>
+  <dimension ref="A1:C55"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43"/>
+      <selection activeCell="C40" sqref="C40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1218,117 +1236,139 @@
         <v>113</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A39" s="5" t="s">
+    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B39" s="4" t="s">
+        <v>117</v>
+      </c>
+      <c r="C39" s="4" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A40" s="3" t="s">
+        <v>116</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="C40" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A41" s="5" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A40" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="3" t="s">
-        <v>69</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>72</v>
       </c>
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A45" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B44" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A45" s="5" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="6" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B48" s="4" t="s">
         <v>93</v>
-      </c>
-    </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>107</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>97</v>
+        <v>94</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>106</v>
+        <v>95</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B55" s="4" t="s">
         <v>102</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Moved to Completed. Attach Docs and write note. Started xcom navigation.
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F49110C-5B05-4A0C-804E-807BA667EDF5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BD6377-B076-4B58-BC20-F23146777E5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="125">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
   <si>
     <t>Name</t>
   </si>
@@ -400,6 +400,109 @@
   </si>
   <si>
     <t>LTRCUST</t>
+  </si>
+  <si>
+    <t>CompletedFolder</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9)Processing Folders\Robot\{1}\Completed\</t>
+  </si>
+  <si>
+    <t>Completed folder path for crfs processed successfully</t>
+  </si>
+  <si>
+    <t>AttachmentNote</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note to be added with last document attached in Customer Notification. 
+</t>
+  </si>
+  <si>
+    <t>Team Leader Name:  Rob Mclean
+Inspection result: 2020 Cross Compliance {0} – {1}
+{2}
+Version of the 2020 Cross Compliance Processing – {3}:
+{4}
+Inspection result Letter/Email Sent: {5}
+CRF and Supporting Documents added to CRM: {6}</t>
+  </si>
+  <si>
+    <t>Version Number of Guidance</t>
+  </si>
+  <si>
+    <t>SAGGuidanceVersion</t>
+  </si>
+  <si>
+    <t>RPAGuidanceVersion</t>
+  </si>
+  <si>
+    <t>CIIGuidanceVersion</t>
+  </si>
+  <si>
+    <t>AWGuidanceVersion</t>
+  </si>
+  <si>
+    <t>AHTBGuidanceVersion</t>
+  </si>
+  <si>
+    <t>SAGInspectionResult</t>
+  </si>
+  <si>
+    <t>RPAInspectionResult</t>
+  </si>
+  <si>
+    <t>CIIInspectionResult</t>
+  </si>
+  <si>
+    <t>AWInspectionResult</t>
+  </si>
+  <si>
+    <t>AHTBInspectionResult</t>
+  </si>
+  <si>
+    <t>Sheep and Goat inspection</t>
+  </si>
+  <si>
+    <t>RPAi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cattle Identification (CII) </t>
+  </si>
+  <si>
+    <t>APHA TB Test</t>
+  </si>
+  <si>
+    <t>Animal Welfare inspection</t>
+  </si>
+  <si>
+    <t>SAGGuidanceTitle</t>
+  </si>
+  <si>
+    <t>AHTBGuidanceTitle</t>
+  </si>
+  <si>
+    <t>AWGuidanceTitle</t>
+  </si>
+  <si>
+    <t>CIIGuidanceTitle</t>
+  </si>
+  <si>
+    <t>RPAGuidanceTitle</t>
+  </si>
+  <si>
+    <t>Sheep and Goat Inspection Instructions</t>
+  </si>
+  <si>
+    <t>Rural Payments Agency Inspection (RPAi) Instructions</t>
+  </si>
+  <si>
+    <t>CII Instructions used</t>
+  </si>
+  <si>
+    <t>APHA Late TB Test Instructions</t>
+  </si>
+  <si>
+    <t>APHA Animal Welfare Inspection Instructions</t>
   </si>
 </sst>
 </file>
@@ -529,8 +632,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C57" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C57" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C74" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C74" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
@@ -837,10 +940,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C57"/>
+  <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
+      <selection activeCell="B59" sqref="B59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1267,130 +1370,260 @@
         <v>121</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A41" s="5" t="s">
+    <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A41" s="3" t="s">
+        <v>125</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="C41" s="4" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A42" s="5" t="s">
         <v>66</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>71</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B46" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A49" s="3" t="s">
         <v>123</v>
       </c>
-      <c r="B48" s="4" t="s">
+      <c r="B49" s="4" t="s">
         <v>124</v>
       </c>
     </row>
-    <row r="49" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
+    <row r="50" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C50" s="4" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
+        <v>137</v>
+      </c>
+      <c r="B51" s="4" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A52" s="3" t="s">
+        <v>138</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
+        <v>139</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A54" s="3" t="s">
+        <v>140</v>
+      </c>
+      <c r="B54" s="4" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A55" s="3" t="s">
+        <v>141</v>
+      </c>
+      <c r="B55" s="4" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>147</v>
+      </c>
+      <c r="B56" s="4" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A57" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B57" s="4" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A58" s="3" t="s">
+        <v>150</v>
+      </c>
+      <c r="B58" s="4" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A59" s="3" t="s">
+        <v>149</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A60" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="B60" s="4" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A61" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A62" s="3" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A63" s="3" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A64" s="3" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A65" s="3" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A66" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="50" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A50" s="6" t="s">
+    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A67" s="6" t="s">
         <v>92</v>
       </c>
-      <c r="B50" s="4" t="s">
+      <c r="B67" s="4" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="51" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
+    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
         <v>94</v>
       </c>
-      <c r="B51" s="4" t="s">
+      <c r="B68" s="4" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="52" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A52" s="3" t="s">
+    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A69" s="3" t="s">
         <v>96</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B69" s="4" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="53" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
+    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A70" s="3" t="s">
         <v>97</v>
       </c>
-      <c r="B53" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="54" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A54" s="3" t="s">
+    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A71" s="3" t="s">
         <v>98</v>
       </c>
-      <c r="B54" s="4" t="s">
+      <c r="B71" s="4" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="55" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
+    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A72" s="3" t="s">
         <v>99</v>
       </c>
-      <c r="B55" s="4" t="s">
+      <c r="B72" s="4" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="56" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A56" s="3" t="s">
+    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A73" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B56" s="4" t="s">
+      <c r="B73" s="4" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="57" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A57" s="3" t="s">
+    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
         <v>101</v>
       </c>
-      <c r="B57" s="4" t="s">
+      <c r="B74" s="4" t="s">
         <v>102</v>
       </c>
     </row>

</xml_diff>

<commit_message>
first day of journey testing, up to crm
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26BD6377-B076-4B58-BC20-F23146777E5E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279D3CA0-6185-4B69-8892-4B9A0408A311}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -942,8 +942,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A51" workbookViewId="0">
-      <selection activeCell="B59" sqref="B59"/>
+    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1534,6 +1534,9 @@
       <c r="A61" s="3" t="s">
         <v>132</v>
       </c>
+      <c r="B61" s="4">
+        <v>1</v>
+      </c>
       <c r="C61" s="4" t="s">
         <v>131</v>
       </c>
@@ -1542,20 +1545,32 @@
       <c r="A62" s="3" t="s">
         <v>133</v>
       </c>
+      <c r="B62" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>134</v>
       </c>
+      <c r="B63" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>135</v>
       </c>
+      <c r="B64" s="4">
+        <v>1</v>
+      </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>136</v>
+      </c>
+      <c r="B65" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Journey tested customer notification and resolving
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{279D3CA0-6185-4B69-8892-4B9A0408A311}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FF9CB8-F4F2-4EFB-82A5-AFC8EFB4DD10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -418,15 +418,6 @@
 </t>
   </si>
   <si>
-    <t>Team Leader Name:  Rob Mclean
-Inspection result: 2020 Cross Compliance {0} – {1}
-{2}
-Version of the 2020 Cross Compliance Processing – {3}:
-{4}
-Inspection result Letter/Email Sent: {5}
-CRF and Supporting Documents added to CRM: {6}</t>
-  </si>
-  <si>
     <t>Version Number of Guidance</t>
   </si>
   <si>
@@ -503,6 +494,20 @@
   </si>
   <si>
     <t>APHA Animal Welfare Inspection Instructions</t>
+  </si>
+  <si>
+    <t>Team Leader Name:  Rob Mclean 
+{0}
+Inspection result: 2020 Cross Compliance {1} – {2}
+{0}
+{3}
+{0}
+Version of the 2020 Cross Compliance Processing – {4}: 
+{5}
+{0}
+Inspection result Letter/Email Sent: {6}
+{0}
+CRF and Supporting Documents added to CRM: {7}</t>
   </si>
 </sst>
 </file>
@@ -942,8 +947,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A55" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1444,7 +1449,7 @@
         <v>128</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>130</v>
+        <v>156</v>
       </c>
       <c r="C50" s="4" t="s">
         <v>129</v>
@@ -1452,98 +1457,98 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B61" s="4">
         <v>1</v>
       </c>
       <c r="C61" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B62" s="4">
         <v>1</v>
@@ -1551,7 +1556,7 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B63" s="4">
         <v>1</v>
@@ -1559,7 +1564,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B64" s="4">
         <v>1</v>
@@ -1567,7 +1572,7 @@
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B65" s="4">
         <v>1</v>

</xml_diff>

<commit_message>
finished invoking ready for journey testing
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
-  <workbookPr defaultThemeVersion="166925"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x952359$\Development\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C5FF9CB8-F4F2-4EFB-82A5-AFC8EFB4DD10}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="157">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
   <si>
     <t>Name</t>
   </si>
@@ -509,11 +508,20 @@
 {0}
 CRF and Supporting Documents added to CRM: {7}</t>
   </si>
+  <si>
+    <t>CustomerUrlRegex</t>
+  </si>
+  <si>
+    <t>.*person\/(\d*)\/permissions</t>
+  </si>
+  <si>
+    <t>Regex to extract the customer number from the RP Url</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -637,12 +645,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C74" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C74" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C75" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C75"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" name="Name" dataDxfId="2"/>
+    <tableColumn id="2" name="Value" dataDxfId="1"/>
+    <tableColumn id="3" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -944,11 +952,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C74"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:C75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
+      <selection activeCell="C77" sqref="C77"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1570,7 +1578,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="65" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>135</v>
       </c>
@@ -1578,12 +1586,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="66" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="6" t="s">
         <v>92</v>
       </c>
@@ -1591,7 +1599,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="68" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>94</v>
       </c>
@@ -1599,7 +1607,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="69" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>96</v>
       </c>
@@ -1607,7 +1615,7 @@
         <v>107</v>
       </c>
     </row>
-    <row r="70" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>97</v>
       </c>
@@ -1615,7 +1623,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="71" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>98</v>
       </c>
@@ -1623,7 +1631,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="72" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>99</v>
       </c>
@@ -1631,7 +1639,7 @@
         <v>104</v>
       </c>
     </row>
-    <row r="73" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>100</v>
       </c>
@@ -1639,12 +1647,23 @@
         <v>103</v>
       </c>
     </row>
-    <row r="74" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>101</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>102</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="3" t="s">
+        <v>157</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C75" s="4" t="s">
+        <v>159</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Journey testing done up to create case. Siti and xcom logic added
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="22527"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x952359$\Development\rpa-future-farming-cross-compliance\Documents\Config\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8A44DC-5908-4243-82D4-23103A70DA05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="160">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
   <si>
     <t>Name</t>
   </si>
@@ -53,9 +54,6 @@
     <t>Path for Robot Processing Folder</t>
   </si>
   <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9)Processing Folders\Robot</t>
-  </si>
-  <si>
     <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\CII Receipting</t>
   </si>
   <si>
@@ -377,15 +375,9 @@
     <t>ReadyToBeReceiptedFolder</t>
   </si>
   <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9)Processing Folders\Robot\{1}\In Progress\</t>
-  </si>
-  <si>
     <t>InProgressWindowFolder</t>
   </si>
   <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9)Processing Folders\Robot\{1}\Ready To Be Receipted\</t>
-  </si>
-  <si>
     <t>in progress path for all crf types</t>
   </si>
   <si>
@@ -402,9 +394,6 @@
   </si>
   <si>
     <t>CompletedFolder</t>
-  </si>
-  <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9)Processing Folders\Robot\{1}\Completed\</t>
   </si>
   <si>
     <t>Completed folder path for crfs processed successfully</t>
@@ -517,11 +506,32 @@
   <si>
     <t>Regex to extract the customer number from the RP Url</t>
   </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9) Processing Folders\Robot</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9) Processing Folders\Robot\{1}\In Progress\</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9) Processing Folders\Robot\{1}\Ready To Be Receipted\</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9) Processing Folders\Robot\{1}\Completed\</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> https://www-chs-perf.ruraldev.org.uk/#/internal_user/dashboard/</t>
+  </si>
+  <si>
+    <t>RPCustomerUrl</t>
+  </si>
+  <si>
+    <t>Url to navigate to the customer details page of the test version of RP</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -645,12 +655,12 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:C75" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C75"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C76" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C76" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
-    <tableColumn id="1" name="Name" dataDxfId="2"/>
-    <tableColumn id="2" name="Value" dataDxfId="1"/>
-    <tableColumn id="3" name="Description" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Description" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -952,11 +962,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C75"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:C76"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="C77" sqref="C77"/>
+    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
+      <selection activeCell="C29" sqref="C28:C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -987,107 +997,107 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>114</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>115</v>
       </c>
       <c r="C3" s="2"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" s="5" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B4" s="2"/>
       <c r="C4" s="2"/>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B5" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C5" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B6" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C6" s="7" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B7" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C7" s="7" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B8" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C8" s="7" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B9" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C9" s="7" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="6" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B10" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" s="6" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B11" s="7" t="b">
         <v>1</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" s="5" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B12" s="2"/>
       <c r="C12" s="2"/>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B13" s="4">
         <v>3</v>
@@ -1096,280 +1106,280 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14" s="3" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B14" s="4">
         <v>1000</v>
       </c>
       <c r="C14" s="7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B15" s="4">
         <v>3000</v>
       </c>
       <c r="C15" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B16" s="4">
         <v>5000</v>
       </c>
       <c r="C16" s="7" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" s="3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B17" s="4">
         <v>30000</v>
       </c>
       <c r="C17" s="7" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B18" s="4">
         <v>60000</v>
       </c>
       <c r="C18" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B19" s="4">
         <v>120000</v>
       </c>
       <c r="C19" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C21" s="7" t="s">
         <v>31</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="C21" s="7" t="s">
-        <v>32</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B22" s="8" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="C22" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B23" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C23" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="B24" s="8" t="s">
         <v>62</v>
       </c>
-      <c r="B24" s="8" t="s">
-        <v>63</v>
-      </c>
       <c r="C24" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B25" s="9" t="s">
         <v>108</v>
       </c>
-      <c r="B25" s="9" t="s">
+      <c r="C25" s="7" t="s">
         <v>109</v>
       </c>
-      <c r="C25" s="7" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" s="5" t="s">
-        <v>29</v>
-      </c>
-      <c r="B26" s="2"/>
-      <c r="C26" s="2"/>
+    </row>
+    <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>162</v>
+      </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="3" t="s">
+      <c r="A27" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="B27" s="2"/>
+      <c r="C27" s="2"/>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B27" s="4" t="s">
+      <c r="B28" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C27" s="4" t="s">
+      <c r="C28" s="4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C28" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>10</v>
+        <v>156</v>
       </c>
       <c r="C29" s="4" t="s">
-        <v>33</v>
+        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>28</v>
+        <v>10</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>27</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>26</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B34" s="4" t="s">
         <v>25</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B35" s="4" t="s">
         <v>24</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
       <c r="B36" s="4" t="s">
         <v>23</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="37" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
-        <v>21</v>
+        <v>13</v>
       </c>
       <c r="B37" s="4" t="s">
         <v>22</v>
       </c>
       <c r="C37" s="4" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
-        <v>111</v>
+        <v>20</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>112</v>
+        <v>21</v>
       </c>
       <c r="C38" s="4" t="s">
-        <v>113</v>
+        <v>40</v>
       </c>
     </row>
     <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="C39" s="4" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1377,55 +1387,58 @@
         <v>116</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>119</v>
+        <v>157</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>125</v>
+        <v>115</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>126</v>
+        <v>158</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>127</v>
-      </c>
-    </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A42" s="5" t="s">
-        <v>66</v>
+        <v>118</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A42" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>159</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B43" s="4" t="s">
-        <v>71</v>
+      <c r="A43" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="B46" s="4" t="s">
         <v>73</v>
@@ -1433,138 +1446,138 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B47" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B48" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="B47" s="4" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="5" t="s">
-        <v>122</v>
-      </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B49" s="4" t="s">
+      <c r="A49" s="5" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A50" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B50" s="4" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="51" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>124</v>
       </c>
-    </row>
-    <row r="50" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A50" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C50" s="4" t="s">
-        <v>129</v>
-      </c>
-    </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A51" s="3" t="s">
-        <v>136</v>
-      </c>
       <c r="B51" s="4" t="s">
-        <v>141</v>
+        <v>152</v>
+      </c>
+      <c r="C51" s="4" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
+        <v>132</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>137</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>142</v>
       </c>
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
+        <v>133</v>
+      </c>
+      <c r="B53" s="4" t="s">
         <v>138</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B54" s="4" t="s">
         <v>139</v>
-      </c>
-      <c r="B54" s="4" t="s">
-        <v>145</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>151</v>
+        <v>140</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>152</v>
+        <v>147</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>153</v>
+        <v>148</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>155</v>
+        <v>149</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>147</v>
+        <v>144</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>131</v>
-      </c>
-      <c r="B61" s="4">
-        <v>1</v>
-      </c>
-      <c r="C61" s="4" t="s">
-        <v>130</v>
+        <v>143</v>
+      </c>
+      <c r="B61" s="4" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>132</v>
+        <v>127</v>
       </c>
       <c r="B62" s="4">
         <v>1</v>
       </c>
+      <c r="C62" s="4" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>133</v>
+        <v>128</v>
       </c>
       <c r="B63" s="4">
         <v>1</v>
@@ -1572,7 +1585,7 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
       <c r="B64" s="4">
         <v>1</v>
@@ -1580,44 +1593,44 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>135</v>
+        <v>130</v>
       </c>
       <c r="B65" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A66" s="5" t="s">
+      <c r="A66" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B66" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A67" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="6" t="s">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B68" s="4" t="s">
         <v>92</v>
-      </c>
-      <c r="B67" s="4" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="3" t="s">
-        <v>94</v>
-      </c>
-      <c r="B68" s="4" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B70" s="4" t="s">
         <v>106</v>
@@ -1625,7 +1638,7 @@
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B71" s="4" t="s">
         <v>105</v>
@@ -1633,7 +1646,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B72" s="4" t="s">
         <v>104</v>
@@ -1641,7 +1654,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="B73" s="4" t="s">
         <v>103</v>
@@ -1649,7 +1662,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="B74" s="4" t="s">
         <v>102</v>
@@ -1657,13 +1670,21 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>157</v>
+        <v>100</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C75" s="4" t="s">
-        <v>159</v>
+        <v>101</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>153</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>154</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Improved date logic, successful testing sag, rpa, aw
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA8A44DC-5908-4243-82D4-23103A70DA05}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79304914-5861-46A5-9CDB-C02F478ECD25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="163" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="167">
   <si>
     <t>Name</t>
   </si>
@@ -519,13 +519,25 @@
     <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9) Processing Folders\Robot\{1}\Completed\</t>
   </si>
   <si>
-    <t xml:space="preserve"> https://www-chs-perf.ruraldev.org.uk/#/internal_user/dashboard/</t>
-  </si>
-  <si>
     <t>RPCustomerUrl</t>
   </si>
   <si>
     <t>Url to navigate to the customer details page of the test version of RP</t>
+  </si>
+  <si>
+    <t>https://www.ruralpayments.service.gov.uk/#/internal_user/dashboard/</t>
+  </si>
+  <si>
+    <t>CaseType</t>
+  </si>
+  <si>
+    <t>Inspections</t>
+  </si>
+  <si>
+    <t>CaseOrigin</t>
+  </si>
+  <si>
+    <t>Internal</t>
   </si>
 </sst>
 </file>
@@ -655,8 +667,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C76" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C76" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C78" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C78" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
@@ -963,10 +975,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C76"/>
+  <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C29" sqref="C28:C29"/>
+    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
+      <selection activeCell="C52" sqref="C52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1234,13 +1246,13 @@
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>160</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>162</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>161</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>160</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>162</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1473,127 +1485,127 @@
         <v>121</v>
       </c>
     </row>
-    <row r="51" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>124</v>
+        <v>165</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C51" s="4" t="s">
-        <v>125</v>
+        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>132</v>
+        <v>163</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>138</v>
+        <v>152</v>
+      </c>
+      <c r="C53" s="4" t="s">
+        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>142</v>
+        <v>135</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>146</v>
+        <v>136</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B62" s="4">
-        <v>1</v>
-      </c>
-      <c r="C62" s="4" t="s">
-        <v>126</v>
+        <v>144</v>
+      </c>
+      <c r="B62" s="4" t="s">
+        <v>151</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B63" s="4">
-        <v>1</v>
+        <v>143</v>
+      </c>
+      <c r="B63" s="4" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B64" s="4">
         <v>1</v>
       </c>
+      <c r="C64" s="4" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B65" s="4">
         <v>1</v>
@@ -1601,89 +1613,105 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B66" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A67" s="5" t="s">
+      <c r="A67" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B67" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A68" s="3" t="s">
+        <v>131</v>
+      </c>
+      <c r="B68" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A69" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A68" s="6" t="s">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A70" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B68" s="4" t="s">
+      <c r="B70" s="4" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B69" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B71" s="4" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B72" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B73" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B75" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B76" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A77" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B75" s="4" t="s">
+      <c r="B77" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="76" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
+    <row r="78" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
         <v>153</v>
       </c>
-      <c r="B76" s="4" t="s">
+      <c r="B78" s="4" t="s">
         <v>154</v>
       </c>
-      <c r="C76" s="4" t="s">
+      <c r="C78" s="4" t="s">
         <v>155</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Receipting details and change status to closed started
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79304914-5861-46A5-9CDB-C02F478ECD25}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10272F1-A33B-4452-93AB-9D6F88D3DDEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -351,9 +351,6 @@
     <t>XcomUrl</t>
   </si>
   <si>
-    <t>http://rpa-domino-dev.dev.azure.defra.cloud/intranet/xcompliance2015.nsf</t>
-  </si>
-  <si>
     <t>Url for Xcom test</t>
   </si>
   <si>
@@ -538,6 +535,9 @@
   </si>
   <si>
     <t>Internal</t>
+  </si>
+  <si>
+    <t>http://d3vmprwldm001.earth.gsi.gov.uk/intranet/xcompliance2020.nsf/</t>
   </si>
 </sst>
 </file>
@@ -977,8 +977,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C78"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A46" workbookViewId="0">
-      <selection activeCell="C52" sqref="C52"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B26" sqref="B26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1009,10 +1009,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>113</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>114</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -1233,26 +1233,26 @@
         <v>64</v>
       </c>
     </row>
-    <row r="25" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>107</v>
       </c>
       <c r="B25" s="9" t="s">
+        <v>166</v>
+      </c>
+      <c r="C25" s="7" t="s">
         <v>108</v>
-      </c>
-      <c r="C25" s="7" t="s">
-        <v>109</v>
       </c>
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>159</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>161</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>160</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>162</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>161</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
@@ -1278,7 +1278,7 @@
         <v>11</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="C29" s="4" t="s">
         <v>8</v>
@@ -1385,46 +1385,46 @@
     </row>
     <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="B39" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>111</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="B40" s="4" t="s">
+        <v>156</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>116</v>
-      </c>
-      <c r="B40" s="4" t="s">
-        <v>157</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>117</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
+        <v>121</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>158</v>
+      </c>
+      <c r="C42" s="4" t="s">
         <v>122</v>
-      </c>
-      <c r="B42" s="4" t="s">
-        <v>159</v>
-      </c>
-      <c r="C42" s="4" t="s">
-        <v>123</v>
       </c>
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
@@ -1474,138 +1474,138 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
+        <v>119</v>
+      </c>
+      <c r="B50" s="4" t="s">
         <v>120</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>121</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B51" s="4" t="s">
         <v>165</v>
-      </c>
-      <c r="B51" s="4" t="s">
-        <v>166</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
+        <v>162</v>
+      </c>
+      <c r="B52" s="4" t="s">
         <v>163</v>
-      </c>
-      <c r="B52" s="4" t="s">
-        <v>164</v>
       </c>
     </row>
     <row r="53" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
+        <v>123</v>
+      </c>
+      <c r="B53" s="4" t="s">
+        <v>151</v>
+      </c>
+      <c r="C53" s="4" t="s">
         <v>124</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>152</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>125</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B64" s="4">
         <v>1</v>
       </c>
       <c r="C64" s="4" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B65" s="4">
         <v>1</v>
@@ -1613,7 +1613,7 @@
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B66" s="4">
         <v>1</v>
@@ -1621,7 +1621,7 @@
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B67" s="4">
         <v>1</v>
@@ -1629,7 +1629,7 @@
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B68" s="4">
         <v>1</v>
@@ -1706,13 +1706,13 @@
     </row>
     <row r="78" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="B78" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="C78" s="4" t="s">
         <v>154</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>155</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
journey tested up to entering compliant details
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B10272F1-A33B-4452-93AB-9D6F88D3DDEF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F751F57F-C3CE-4182-8886-B43BC52AF054}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="167">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
   <si>
     <t>Name</t>
   </si>
@@ -538,6 +538,39 @@
   </si>
   <si>
     <t>http://d3vmprwldm001.earth.gsi.gov.uk/intranet/xcompliance2020.nsf/</t>
+  </si>
+  <si>
+    <t>SharepointURL</t>
+  </si>
+  <si>
+    <t>SharepointFilePath</t>
+  </si>
+  <si>
+    <t>/UserInstructions/XC%20Master%20List%202021%20v1.0.xlsx</t>
+  </si>
+  <si>
+    <t>Item URL for Legacy LookUp document on Sharepoint</t>
+  </si>
+  <si>
+    <t>https://defra.sharepoint.com/teams/Team1140</t>
+  </si>
+  <si>
+    <t>URL for Defra Sharepoint for legacy Look Up document</t>
+  </si>
+  <si>
+    <t>LegacyLookUpFilePath</t>
+  </si>
+  <si>
+    <t>File path to save Legacy Look up file to from Sharepoint</t>
+  </si>
+  <si>
+    <t>C:\Users\{0}\Desktop\</t>
+  </si>
+  <si>
+    <t>LegacyLookUpSavePath</t>
+  </si>
+  <si>
+    <t>C:\Users\{0}\Desktop\XC Master list 2021 v1.0.xlsx</t>
   </si>
 </sst>
 </file>
@@ -667,8 +700,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C78" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C78" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C82" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C82" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
@@ -975,10 +1008,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C78"/>
+  <dimension ref="A1:C82"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B26" sqref="B26"/>
+    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+      <selection activeCell="F52" sqref="F52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1255,463 +1288,504 @@
         <v>160</v>
       </c>
     </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" s="5" t="s">
+    <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B27" s="9" t="s">
+        <v>171</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A28" s="5" t="s">
         <v>28</v>
       </c>
-      <c r="B27" s="2"/>
-      <c r="C27" s="2"/>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" s="3" t="s">
+      <c r="B28" s="2"/>
+      <c r="C28" s="2"/>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A29" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B28" s="4" t="s">
+      <c r="B29" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C28" s="4" t="s">
+      <c r="C29" s="4" t="s">
         <v>6</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>155</v>
-      </c>
-      <c r="C29" s="4" t="s">
-        <v>8</v>
       </c>
     </row>
     <row r="30" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="3" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>9</v>
+        <v>155</v>
       </c>
       <c r="C30" s="4" t="s">
-        <v>32</v>
+        <v>8</v>
       </c>
     </row>
     <row r="31" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C31" s="4" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="32" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>27</v>
+        <v>10</v>
       </c>
       <c r="C32" s="4" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="33" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="C33" s="4" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="34" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C34" s="4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C35" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="C36" s="4" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B37" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C37" s="4" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A38" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B37" s="4" t="s">
+      <c r="B38" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="C37" s="4" t="s">
+      <c r="C38" s="4" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="38" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A38" s="3" t="s">
+    <row r="39" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A39" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B38" s="4" t="s">
+      <c r="B39" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C39" s="4" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="39" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A39" s="3" t="s">
-        <v>109</v>
-      </c>
-      <c r="B39" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="C39" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="40" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>156</v>
+        <v>110</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B42" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C42" s="4" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A43" s="3" t="s">
         <v>121</v>
       </c>
-      <c r="B42" s="4" t="s">
+      <c r="B43" s="4" t="s">
         <v>158</v>
       </c>
-      <c r="C42" s="4" t="s">
+      <c r="C43" s="4" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>66</v>
+        <v>168</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
+        <v>169</v>
+      </c>
+      <c r="C44" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
-        <v>68</v>
+        <v>173</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>71</v>
+        <v>177</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>174</v>
       </c>
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>69</v>
+        <v>176</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>73</v>
+        <v>175</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="B47" s="4" t="s">
-        <v>72</v>
+      <c r="A47" s="5" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
-        <v>74</v>
+        <v>66</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>75</v>
+        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A49" s="5" t="s">
-        <v>118</v>
+      <c r="A49" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="B49" s="4" t="s">
+        <v>71</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>119</v>
+        <v>69</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>120</v>
+        <v>73</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>164</v>
+        <v>67</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>165</v>
+        <v>72</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
-        <v>162</v>
+        <v>74</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" ht="180" x14ac:dyDescent="0.25">
-      <c r="A53" s="3" t="s">
-        <v>123</v>
-      </c>
-      <c r="B53" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>124</v>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>131</v>
+        <v>119</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>136</v>
+        <v>120</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="3" t="s">
-        <v>132</v>
+        <v>164</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>137</v>
+        <v>165</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>134</v>
+        <v>123</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>140</v>
+        <v>151</v>
+      </c>
+      <c r="C57" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>144</v>
+        <v>134</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>143</v>
+        <v>135</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>150</v>
+        <v>139</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B64" s="4">
-        <v>1</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>125</v>
+        <v>145</v>
+      </c>
+      <c r="B64" s="4" t="s">
+        <v>147</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B65" s="4">
-        <v>1</v>
+        <v>144</v>
+      </c>
+      <c r="B65" s="4" t="s">
+        <v>148</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B66" s="4">
-        <v>1</v>
+        <v>143</v>
+      </c>
+      <c r="B66" s="4" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B67" s="4">
-        <v>1</v>
+        <v>142</v>
+      </c>
+      <c r="B67" s="4" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="B68" s="4">
         <v>1</v>
       </c>
+      <c r="C68" s="4" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A69" s="5" t="s">
-        <v>4</v>
+      <c r="A69" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B69" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A70" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="B70" s="4" t="s">
-        <v>92</v>
+      <c r="A70" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B70" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B71" s="4" t="s">
-        <v>94</v>
+        <v>129</v>
+      </c>
+      <c r="B71" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B72" s="4" t="s">
-        <v>106</v>
+        <v>130</v>
+      </c>
+      <c r="B72" s="4">
+        <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="3" t="s">
-        <v>96</v>
-      </c>
-      <c r="B73" s="4" t="s">
-        <v>105</v>
+      <c r="A73" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="3" t="s">
-        <v>97</v>
+      <c r="A74" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="B74" s="4" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="3" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
       <c r="B75" s="4" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>102</v>
+        <v>106</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B77" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A78" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B78" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A79" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B79" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A80" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B80" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B77" s="4" t="s">
+      <c r="B81" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="78" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="3" t="s">
+    <row r="82" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B78" s="4" t="s">
+      <c r="B82" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C78" s="4" t="s">
+      <c r="C82" s="4" t="s">
         <v>154</v>
       </c>
     </row>

</xml_diff>

<commit_message>
ran whole way through - redid input contact in crm, added in exception folder to logic, move sbi folder to application year
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F751F57F-C3CE-4182-8886-B43BC52AF054}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DA4350-F25E-4FCC-BAFA-34080389C7A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="178" uniqueCount="178">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
   <si>
     <t>Name</t>
   </si>
@@ -571,6 +571,18 @@
   </si>
   <si>
     <t>C:\Users\{0}\Desktop\XC Master list 2021 v1.0.xlsx</t>
+  </si>
+  <si>
+    <t>ExceptionsFolder</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\9) Processing Folders\Robot\{1}\Exceptions</t>
+  </si>
+  <si>
+    <t>outlookExceptionsFolder</t>
+  </si>
+  <si>
+    <t>Exceptions</t>
   </si>
 </sst>
 </file>
@@ -700,8 +712,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C82" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C82" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C84" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C84" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
@@ -1008,10 +1020,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C82"/>
+  <dimension ref="A1:C84"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="F52" sqref="F52"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="A43" activeCellId="1" sqref="A54:XFD54 A43:XFD43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1462,240 +1474,240 @@
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>121</v>
+        <v>178</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C43" s="4" t="s">
-        <v>122</v>
+        <v>179</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
-        <v>168</v>
+        <v>121</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>170</v>
+        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>168</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>169</v>
+      </c>
+      <c r="C45" s="4" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A46" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="B45" s="4" t="s">
+      <c r="B46" s="4" t="s">
         <v>177</v>
       </c>
-      <c r="C45" s="4" t="s">
+      <c r="C46" s="4" t="s">
         <v>174</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A46" s="3" t="s">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A47" s="3" t="s">
         <v>176</v>
       </c>
-      <c r="B46" s="4" t="s">
+      <c r="B47" s="4" t="s">
         <v>175</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A47" s="5" t="s">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A48" s="5" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A48" s="3" t="s">
-        <v>66</v>
-      </c>
-      <c r="B48" s="4" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="3" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="B52" s="4" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A53" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B52" s="4" t="s">
+      <c r="B53" s="4" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A53" s="5" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>119</v>
+        <v>180</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>120</v>
+        <v>181</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A55" s="3" t="s">
-        <v>164</v>
-      </c>
-      <c r="B55" s="4" t="s">
-        <v>165</v>
+      <c r="A55" s="5" t="s">
+        <v>118</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
-        <v>162</v>
+        <v>119</v>
       </c>
       <c r="B56" s="4" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="57" spans="1:3" ht="180" x14ac:dyDescent="0.25">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
-        <v>123</v>
+        <v>164</v>
       </c>
       <c r="B57" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>124</v>
+        <v>165</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
-        <v>131</v>
+        <v>162</v>
       </c>
       <c r="B58" s="4" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="59" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="B59" s="4" t="s">
-        <v>137</v>
+        <v>151</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>145</v>
+        <v>135</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>126</v>
-      </c>
-      <c r="B68" s="4">
-        <v>1</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>125</v>
+        <v>143</v>
+      </c>
+      <c r="B68" s="4" t="s">
+        <v>150</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>127</v>
-      </c>
-      <c r="B69" s="4">
-        <v>1</v>
+        <v>142</v>
+      </c>
+      <c r="B69" s="4" t="s">
+        <v>149</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B70" s="4">
         <v>1</v>
       </c>
+      <c r="C70" s="4" t="s">
+        <v>125</v>
+      </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B71" s="4">
         <v>1</v>
@@ -1703,89 +1715,105 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="B72" s="4">
         <v>1</v>
       </c>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A73" s="5" t="s">
+      <c r="A73" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B73" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A74" s="3" t="s">
+        <v>130</v>
+      </c>
+      <c r="B74" s="4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A75" s="5" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A74" s="6" t="s">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A76" s="6" t="s">
         <v>91</v>
       </c>
-      <c r="B74" s="4" t="s">
+      <c r="B76" s="4" t="s">
         <v>92</v>
-      </c>
-    </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A75" s="3" t="s">
-        <v>93</v>
-      </c>
-      <c r="B75" s="4" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="B76" s="4" t="s">
-        <v>106</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>96</v>
+        <v>93</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>105</v>
+        <v>94</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B81" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A82" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B82" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B81" s="4" t="s">
+      <c r="B83" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="82" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
+    <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B82" s="4" t="s">
+      <c r="B84" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C82" s="4" t="s">
+      <c r="C84" s="4" t="s">
         <v>154</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Added comment to xcom and crm, added mi note to logfile
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -8,24 +8,32 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4DA4350-F25E-4FCC-BAFA-34080389C7A3}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9026C0D2-F7B2-4A68-BD5B-5FB7B331CC1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="182" uniqueCount="182">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="195" uniqueCount="195">
   <si>
     <t>Name</t>
   </si>
@@ -583,6 +591,47 @@
   </si>
   <si>
     <t>Exceptions</t>
+  </si>
+  <si>
+    <t>XcomComment</t>
+  </si>
+  <si>
+    <t>The comment to be entered in to XCOM and the note in CRM. For compliant only.</t>
+  </si>
+  <si>
+    <t>XCOM Info</t>
+  </si>
+  <si>
+    <t>Sheep and Goats Inspection</t>
+  </si>
+  <si>
+    <t>SAGInspectionName</t>
+  </si>
+  <si>
+    <t>RPAInspectionName</t>
+  </si>
+  <si>
+    <t>CIIInspectionName</t>
+  </si>
+  <si>
+    <t>AWInspectionName</t>
+  </si>
+  <si>
+    <t>Rural Payments Agency Inspection</t>
+  </si>
+  <si>
+    <t>Cattle Identification Inspection</t>
+  </si>
+  <si>
+    <t>Animal Welfare Inspection</t>
+  </si>
+  <si>
+    <t>Used in the XcomComment</t>
+  </si>
+  <si>
+    <t>Cross Compliance {1}{0}
+{2}
+{3}</t>
   </si>
 </sst>
 </file>
@@ -712,8 +761,8 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C84" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A1:C84" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:C90" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A1:C90" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Name" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Value" dataDxfId="1"/>
@@ -1020,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C84"/>
+  <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="A43" activeCellId="1" sqref="A54:XFD54 A43:XFD43"/>
+    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
+      <selection activeCell="D76" sqref="D76"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1739,81 +1788,132 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A76" s="6" t="s">
-        <v>91</v>
+        <v>184</v>
+      </c>
+    </row>
+    <row r="76" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A76" s="3" t="s">
+        <v>182</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>92</v>
+        <v>194</v>
+      </c>
+      <c r="C76" s="4" t="s">
+        <v>183</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>93</v>
+        <v>186</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>94</v>
+        <v>185</v>
+      </c>
+      <c r="C77" s="4" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
-        <v>95</v>
+        <v>187</v>
       </c>
       <c r="B78" s="4" t="s">
-        <v>106</v>
+        <v>190</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
-        <v>96</v>
+        <v>188</v>
       </c>
       <c r="B79" s="4" t="s">
-        <v>105</v>
+        <v>191</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
-        <v>97</v>
+        <v>189</v>
       </c>
       <c r="B80" s="4" t="s">
-        <v>104</v>
+        <v>192</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>98</v>
-      </c>
-      <c r="B81" s="4" t="s">
-        <v>103</v>
+      <c r="A81" s="5" t="s">
+        <v>4</v>
       </c>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A82" s="3" t="s">
-        <v>99</v>
+      <c r="A82" s="6" t="s">
+        <v>91</v>
       </c>
       <c r="B82" s="4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="B83" s="4" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
+        <v>95</v>
+      </c>
+      <c r="B84" s="4" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="B85" s="4" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="B86" s="4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="B87" s="4" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A88" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="B88" s="4" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A89" s="3" t="s">
         <v>100</v>
       </c>
-      <c r="B83" s="4" t="s">
+      <c r="B89" s="4" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="84" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
+    <row r="90" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A90" s="3" t="s">
         <v>152</v>
       </c>
-      <c r="B84" s="4" t="s">
+      <c r="B90" s="4" t="s">
         <v>153</v>
       </c>
-      <c r="C84" s="4" t="s">
+      <c r="C90" s="4" t="s">
         <v>154</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Journey tested RPA and AH
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9026C0D2-F7B2-4A68-BD5B-5FB7B331CC1D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAE0E2A-BFD4-44AA-B0F6-D5833CAEE04C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="105" yWindow="2685" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -365,9 +365,6 @@
     <t>CPHLinkLookUp</t>
   </si>
   <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance 2020\2020 SBI_CPH Link\2020 SBI_CPH Link.xls</t>
-  </si>
-  <si>
     <t>folder path to cph link up sbi</t>
   </si>
   <si>
@@ -554,9 +551,6 @@
     <t>SharepointFilePath</t>
   </si>
   <si>
-    <t>/UserInstructions/XC%20Master%20List%202021%20v1.0.xlsx</t>
-  </si>
-  <si>
     <t>Item URL for Legacy LookUp document on Sharepoint</t>
   </si>
   <si>
@@ -576,9 +570,6 @@
   </si>
   <si>
     <t>LegacyLookUpSavePath</t>
-  </si>
-  <si>
-    <t>C:\Users\{0}\Desktop\XC Master list 2021 v1.0.xlsx</t>
   </si>
   <si>
     <t>ExceptionsFolder</t>
@@ -632,6 +623,15 @@
     <t>Cross Compliance {1}{0}
 {2}
 {3}</t>
+  </si>
+  <si>
+    <t>/UserInstructions/XC%20Master%20List%20{0}%20v1.0.xlsx</t>
+  </si>
+  <si>
+    <t>C:\Users\{0}\Desktop\XC Master list {1} v1.0.xlsx</t>
+  </si>
+  <si>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\{0} SBI_CPH Link\2020 SBI_CPH Link.xls</t>
   </si>
 </sst>
 </file>
@@ -1071,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A64" workbookViewId="0">
-      <selection activeCell="D76" sqref="D76"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B30" sqref="B30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1103,10 +1103,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="7" t="s">
         <v>112</v>
-      </c>
-      <c r="B3" s="7" t="s">
-        <v>113</v>
       </c>
       <c r="C3" s="2"/>
     </row>
@@ -1332,7 +1332,7 @@
         <v>107</v>
       </c>
       <c r="B25" s="9" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>108</v>
@@ -1340,24 +1340,24 @@
     </row>
     <row r="26" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
+        <v>158</v>
+      </c>
+      <c r="B26" s="9" t="s">
+        <v>160</v>
+      </c>
+      <c r="C26" s="7" t="s">
         <v>159</v>
-      </c>
-      <c r="B26" s="9" t="s">
-        <v>161</v>
-      </c>
-      <c r="C26" s="7" t="s">
-        <v>160</v>
       </c>
     </row>
     <row r="27" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B27" s="9" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="C27" s="7" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
@@ -1383,7 +1383,7 @@
         <v>11</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C30" s="4" t="s">
         <v>8</v>
@@ -1493,81 +1493,81 @@
         <v>109</v>
       </c>
       <c r="B40" s="4" t="s">
+        <v>194</v>
+      </c>
+      <c r="C40" s="4" t="s">
         <v>110</v>
-      </c>
-      <c r="C40" s="4" t="s">
-        <v>111</v>
       </c>
     </row>
     <row r="41" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="B41" s="4" t="s">
+        <v>155</v>
+      </c>
+      <c r="C41" s="4" t="s">
         <v>115</v>
-      </c>
-      <c r="B41" s="4" t="s">
-        <v>156</v>
-      </c>
-      <c r="C41" s="4" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="42" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="43" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
     </row>
     <row r="44" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
+        <v>120</v>
+      </c>
+      <c r="B44" s="4" t="s">
+        <v>157</v>
+      </c>
+      <c r="C44" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="B44" s="4" t="s">
-        <v>158</v>
-      </c>
-      <c r="C44" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="45" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
+        <v>167</v>
+      </c>
+      <c r="B45" s="4" t="s">
+        <v>192</v>
+      </c>
+      <c r="C45" s="4" t="s">
         <v>168</v>
-      </c>
-      <c r="B45" s="4" t="s">
-        <v>169</v>
-      </c>
-      <c r="C45" s="4" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="46" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A46" s="3" t="s">
-        <v>173</v>
+        <v>171</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>177</v>
+        <v>193</v>
       </c>
       <c r="C46" s="4" t="s">
-        <v>174</v>
+        <v>172</v>
       </c>
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
-        <v>176</v>
+        <v>174</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>175</v>
+        <v>173</v>
       </c>
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
@@ -1617,146 +1617,146 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="5" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
+        <v>118</v>
+      </c>
+      <c r="B56" s="4" t="s">
         <v>119</v>
-      </c>
-      <c r="B56" s="4" t="s">
-        <v>120</v>
       </c>
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
+        <v>163</v>
+      </c>
+      <c r="B57" s="4" t="s">
         <v>164</v>
-      </c>
-      <c r="B57" s="4" t="s">
-        <v>165</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="3" t="s">
+        <v>161</v>
+      </c>
+      <c r="B58" s="4" t="s">
         <v>162</v>
-      </c>
-      <c r="B58" s="4" t="s">
-        <v>163</v>
       </c>
     </row>
     <row r="59" spans="1:3" ht="180" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
+        <v>122</v>
+      </c>
+      <c r="B59" s="4" t="s">
+        <v>150</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>123</v>
-      </c>
-      <c r="B59" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="C59" s="4" t="s">
-        <v>124</v>
       </c>
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B60" s="4" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B63" s="4" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B64" s="4" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B69" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B70" s="4">
         <v>1</v>
       </c>
       <c r="C70" s="4" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B71" s="4">
         <v>1</v>
@@ -1764,7 +1764,7 @@
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B72" s="4">
         <v>1</v>
@@ -1772,7 +1772,7 @@
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B73" s="4">
         <v>1</v>
@@ -1780,7 +1780,7 @@
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B74" s="4">
         <v>1</v>
@@ -1788,53 +1788,53 @@
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="5" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
     </row>
     <row r="76" spans="1:3" ht="45" x14ac:dyDescent="0.25">
       <c r="A76" s="3" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="B76" s="4" t="s">
-        <v>194</v>
+        <v>191</v>
       </c>
       <c r="C76" s="4" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="3" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="B77" s="4" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="C77" s="4" t="s">
-        <v>193</v>
+        <v>190</v>
       </c>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="3" t="s">
+        <v>184</v>
+      </c>
+      <c r="B78" s="4" t="s">
         <v>187</v>
-      </c>
-      <c r="B78" s="4" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="3" t="s">
+        <v>185</v>
+      </c>
+      <c r="B79" s="4" t="s">
         <v>188</v>
-      </c>
-      <c r="B79" s="4" t="s">
-        <v>191</v>
       </c>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="3" t="s">
+        <v>186</v>
+      </c>
+      <c r="B80" s="4" t="s">
         <v>189</v>
-      </c>
-      <c r="B80" s="4" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.25">
@@ -1908,13 +1908,13 @@
     </row>
     <row r="90" spans="1:3" ht="30" x14ac:dyDescent="0.25">
       <c r="A90" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="B90" s="4" t="s">
         <v>152</v>
       </c>
-      <c r="B90" s="4" t="s">
+      <c r="C90" s="4" t="s">
         <v>153</v>
-      </c>
-      <c r="C90" s="4" t="s">
-        <v>154</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Change to configs for SBI look up path, and crm selector change
</commit_message>
<xml_diff>
--- a/Documents/Config/config.xlsx
+++ b/Documents/Config/config.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\GFD218DF\x953922$\UiPath\rpa-future-farming-cross-compliance\Documents\Config\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FAE0E2A-BFD4-44AA-B0F6-D5833CAEE04C}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3B86C77-8395-44C1-8A8A-ABBF02AE31E9}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="105" yWindow="2685" windowWidth="15375" windowHeight="7875" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -631,7 +631,7 @@
     <t>C:\Users\{0}\Desktop\XC Master list {1} v1.0.xlsx</t>
   </si>
   <si>
-    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\{0} SBI_CPH Link\2020 SBI_CPH Link.xls</t>
+    <t>\\cavmfil001\Common\SinglePaymentScheme\Cross Compliance {0}\{0} SBI_CPH Link\2020 SBI_CPH Link.xlsx</t>
   </si>
 </sst>
 </file>
@@ -1071,8 +1071,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C90"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="B30" sqref="B30"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>